<commit_message>
Added assign leave functionality
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/ExcelTestData.xlsx
+++ b/src/main/resources/testdata/ExcelTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anupamadhir/workspace/orangehrm/src/main/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D21079E-ECFE-ED4F-9C79-25DDB5255DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA59D24D-476B-8140-A129-F28DEEB1C302}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10360" yWindow="4060" windowWidth="28040" windowHeight="15940" xr2:uid="{F68E6180-9A72-D840-8501-FC2956D32866}"/>
   </bookViews>
@@ -32,16 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
-  <si>
-    <t>test_method_name</t>
-  </si>
-  <si>
-    <t>data 2</t>
-  </si>
-  <si>
-    <t>sample data 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>add_leave_entitlement</t>
   </si>
@@ -71,12 +62,24 @@
   </si>
   <si>
     <t>Russel Hamilton</t>
+  </si>
+  <si>
+    <t>From Date</t>
+  </si>
+  <si>
+    <t>To Date</t>
+  </si>
+  <si>
+    <t>assign_leave</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="12"/>
@@ -125,12 +128,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB8815C-C7F8-2E45-BD25-BC17A7749A87}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -462,77 +466,90 @@
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" s="2" t="s">
+      <c r="D7" s="5">
+        <v>43994</v>
+      </c>
+      <c r="E7" s="5">
+        <v>44001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="F8" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="F9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="F10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="G11" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>